<commit_message>
Adds missing topics in Excel file; Fixes bug
</commit_message>
<xml_diff>
--- a/havoa.xlsx
+++ b/havoa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bertjan/Projects/examenfit/api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21505B67-295E-124E-BB6E-FA4D1C0C2DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88120887-E068-D941-A787-FBBF31A58FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="500" windowWidth="33600" windowHeight="37300" xr2:uid="{E99334D0-8409-004C-9D3A-53BC8AECB376}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1852" uniqueCount="401">
   <si>
     <t>Opgave</t>
   </si>
@@ -1357,6 +1357,210 @@
   </si>
   <si>
     <t>Slaaponderzoek bij de San</t>
+  </si>
+  <si>
+    <t>Akkerranden</t>
+  </si>
+  <si>
+    <t>B1: Rekenen
+C1: Tabellen</t>
+  </si>
+  <si>
+    <t>Tabel
+Eenheden
+Verhouding</t>
+  </si>
+  <si>
+    <t>Oppervlakte berekenen, gegevens uit tekst en tabel combineren en rekenen, uitkomst vergelijken met waarde</t>
+  </si>
+  <si>
+    <t>Lineair verband
+Meer dan twee variabelen
+Grafische rekenmachine
+Vergelijking
+Afronden</t>
+  </si>
+  <si>
+    <t>Waarde invullen in formule, vergelijking oplossen (GR)</t>
+  </si>
+  <si>
+    <t>B2: Algebra
+C3: Formules en vergelijkingen
+C4: Lineaire verbanden</t>
+  </si>
+  <si>
+    <t>Lineair verband
+Meer dan twee variabelen
+Herleiden</t>
+  </si>
+  <si>
+    <t>Waarde invullen in formule, variabele vrij maken in lineaire vergelijking</t>
+  </si>
+  <si>
+    <t>Onderzoek naar rekenvaardigheid</t>
+  </si>
+  <si>
+    <t>Staafdiagram/histogram
+Statistische visualisatie
+Conclusies
+Redeneren
+Gemiddelde</t>
+  </si>
+  <si>
+    <t>Redeneren over gemiddelde aan de hand van staafdiagram</t>
+  </si>
+  <si>
+    <t>C1: Tabellen
+E3: Data en verdelingen</t>
+  </si>
+  <si>
+    <t>Tabel
+Normale verdeling</t>
+  </si>
+  <si>
+    <t>Beredeneren of een variabele normaal verdeeld is aan de hand van tabel</t>
+  </si>
+  <si>
+    <t>Bepaal</t>
+  </si>
+  <si>
+    <t>Tabel
+Groepen vergelijken
+Boxplots vergelijken
+Boxplot
+Effectgrootte</t>
+  </si>
+  <si>
+    <t>Methodes voor groepen vergelijken kiezen, effectgrootte berekenen, boxplots maken en vergelijken</t>
+  </si>
+  <si>
+    <t>Tabel
+Spreiding
+Standaardafwijking
+Kwartielafspraak</t>
+  </si>
+  <si>
+    <t>Twee spreidingsmaten kiezen, spreiding vergelijken</t>
+  </si>
+  <si>
+    <t>Grafiek
+Spreiding</t>
+  </si>
+  <si>
+    <t>Spreidingsmaat kiezen, spreiding van twee scores vergelijken</t>
+  </si>
+  <si>
+    <t>Great Barrier Reef</t>
+  </si>
+  <si>
+    <t>Procentuele verandering
+Afronden</t>
+  </si>
+  <si>
+    <t>Gegevens uit tekst verwerken, procentuele verandering berekenen</t>
+  </si>
+  <si>
+    <t>Groeifactor omrekenen naar andere tijdseenheid, omrekenen naar groeipercentage</t>
+  </si>
+  <si>
+    <t>Groeifactor
+Exponentieel verband
+Vergelijking
+Grafische rekenmachine
+Verdubbelingstijd</t>
+  </si>
+  <si>
+    <t>Groeifactor bepalen, vergelijking opstellen, oplossen (GR)</t>
+  </si>
+  <si>
+    <t>Studieschuld</t>
+  </si>
+  <si>
+    <t>Groeifactor
+Afronden</t>
+  </si>
+  <si>
+    <t>Groeifactor omrekenen naar andere tijdseenheid</t>
+  </si>
+  <si>
+    <t>Exponentieel verband
+Vergelijking
+Grafische rekenmachine</t>
+  </si>
+  <si>
+    <t>Waarde invullen, vergelijking oplossen (GR)</t>
+  </si>
+  <si>
+    <t>Tabel</t>
+  </si>
+  <si>
+    <t>Waarde in tabel aflezen</t>
+  </si>
+  <si>
+    <t>Tabel
+Lineair verband
+Lineaire inter-/extrapoleren
+Richtingscoëfficiënt</t>
+  </si>
+  <si>
+    <t>Twee waarden uit tabel aflezen, lineair interpoleren</t>
+  </si>
+  <si>
+    <t>Papierformaten</t>
+  </si>
+  <si>
+    <t>Tabel
+Exponentieel verband
+Groeifactor</t>
+  </si>
+  <si>
+    <t>Waarde uit tabel halen, hoeveelheid 11 keer halveren</t>
+  </si>
+  <si>
+    <t>Substitutie
+Grafische rekenmachine
+Afronden
+Vergelijking</t>
+  </si>
+  <si>
+    <t>Twee formules combineren, waarde invullen, vergelijking oplossen (GR), conclusie trekken</t>
+  </si>
+  <si>
+    <t>Exponentieel verband aantonen door groeifactoren te vergelijken</t>
+  </si>
+  <si>
+    <t>Lineair verband
+Lineair inter-/extrapoleren</t>
+  </si>
+  <si>
+    <t>Stapgrootte bepalen, extrapoleren</t>
+  </si>
+  <si>
+    <t>Lineaire formule opstellen
+Lineair verband
+Richtingscoëfficiënt</t>
+  </si>
+  <si>
+    <t>Parameters in lineaire formule bepalen</t>
+  </si>
+  <si>
+    <t>Bioscoopbezoek</t>
+  </si>
+  <si>
+    <t>C1: Tabellen
+C2: Grafieken</t>
+  </si>
+  <si>
+    <t>Gemiddelde
+Meer dan twee variabelen
+Tabel
+Staafdiagram/histogram
+Statistische visualisatie
+Lijndiagram/frequentiepolygoon
+Redeneren</t>
+  </si>
+  <si>
+    <t>Juiste gegeven uit tabel halen, Gegevens verwerken uit tekst, lijndiagram en staafdiagram, rekenen met gemiddelde</t>
   </si>
 </sst>
 </file>
@@ -1760,10 +1964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D78E083-C8D6-F941-BBFE-10A211561DB0}">
-  <dimension ref="A1:R129"/>
+  <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B42" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
+      <selection activeCell="N130" sqref="N130:N151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7273,7 +7477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="34" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>343</v>
       </c>
@@ -7310,6 +7514,816 @@
       <c r="L129" s="9" t="s">
         <v>75</v>
       </c>
+    </row>
+    <row r="130" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>350</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>47</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="G130" t="s">
+        <v>35</v>
+      </c>
+      <c r="H130" t="s">
+        <v>18</v>
+      </c>
+      <c r="I130" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J130" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K130" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L130" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N130" s="5"/>
+    </row>
+    <row r="131" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
+        <v>13</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="G131" t="s">
+        <v>44</v>
+      </c>
+      <c r="H131" t="s">
+        <v>31</v>
+      </c>
+      <c r="I131" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J131" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K131" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L131" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N131" s="5"/>
+    </row>
+    <row r="132" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>3</v>
+      </c>
+      <c r="C132" t="s">
+        <v>13</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G132" t="s">
+        <v>17</v>
+      </c>
+      <c r="H132" t="s">
+        <v>31</v>
+      </c>
+      <c r="I132" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J132" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K132" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L132" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N132" s="5"/>
+    </row>
+    <row r="133" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>4</v>
+      </c>
+      <c r="C133" t="s">
+        <v>40</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="G133" t="s">
+        <v>25</v>
+      </c>
+      <c r="H133" t="s">
+        <v>26</v>
+      </c>
+      <c r="I133" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J133" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K133" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L133" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N133" s="5"/>
+    </row>
+    <row r="134" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>359</v>
+      </c>
+      <c r="B134">
+        <v>5</v>
+      </c>
+      <c r="C134" t="s">
+        <v>68</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="G134" t="s">
+        <v>61</v>
+      </c>
+      <c r="H134" t="s">
+        <v>55</v>
+      </c>
+      <c r="I134" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J134" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K134" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L134" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N134" s="5"/>
+    </row>
+    <row r="135" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>6</v>
+      </c>
+      <c r="C135" t="s">
+        <v>68</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G135" t="s">
+        <v>54</v>
+      </c>
+      <c r="H135" t="s">
+        <v>55</v>
+      </c>
+      <c r="I135" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="J135" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K135" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L135" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N135" s="5"/>
+    </row>
+    <row r="136" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>7</v>
+      </c>
+      <c r="C136" t="s">
+        <v>365</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="G136" t="s">
+        <v>132</v>
+      </c>
+      <c r="H136" t="s">
+        <v>55</v>
+      </c>
+      <c r="I136" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J136" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K136" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L136" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N136" s="5"/>
+    </row>
+    <row r="137" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>8</v>
+      </c>
+      <c r="C137" t="s">
+        <v>68</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="G137" t="s">
+        <v>61</v>
+      </c>
+      <c r="H137" t="s">
+        <v>55</v>
+      </c>
+      <c r="I137" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J137" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K137" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L137" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N137" s="5"/>
+    </row>
+    <row r="138" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>9</v>
+      </c>
+      <c r="C138" t="s">
+        <v>68</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G138" t="s">
+        <v>61</v>
+      </c>
+      <c r="H138" t="s">
+        <v>55</v>
+      </c>
+      <c r="I138" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J138" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K138" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="L138" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N138" s="5"/>
+    </row>
+    <row r="139" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>372</v>
+      </c>
+      <c r="B139">
+        <v>10</v>
+      </c>
+      <c r="C139" t="s">
+        <v>13</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E139" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="G139" t="s">
+        <v>17</v>
+      </c>
+      <c r="H139" t="s">
+        <v>18</v>
+      </c>
+      <c r="I139" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J139" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K139" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L139" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N139" s="5"/>
+    </row>
+    <row r="140" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>11</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I140" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J140" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K140" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L140" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N140" s="5"/>
+    </row>
+    <row r="141" spans="1:14" ht="85" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>12</v>
+      </c>
+      <c r="C141" t="s">
+        <v>13</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="G141" t="s">
+        <v>78</v>
+      </c>
+      <c r="H141" t="s">
+        <v>91</v>
+      </c>
+      <c r="I141" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J141" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K141" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L141" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N141" s="5"/>
+    </row>
+    <row r="142" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>378</v>
+      </c>
+      <c r="B142">
+        <v>13</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E142" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="F142" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I142" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J142" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K142" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L142" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N142" s="5"/>
+    </row>
+    <row r="143" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>14</v>
+      </c>
+      <c r="C143" t="s">
+        <v>13</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="G143" t="s">
+        <v>78</v>
+      </c>
+      <c r="H143" t="s">
+        <v>91</v>
+      </c>
+      <c r="I143" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J143" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K143" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L143" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N143" s="5"/>
+    </row>
+    <row r="144" spans="1:14" ht="17" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>15</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="F144" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I144" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J144" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K144" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L144" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N144" s="5"/>
+    </row>
+    <row r="145" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>16</v>
+      </c>
+      <c r="C145" t="s">
+        <v>13</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="G145" t="s">
+        <v>25</v>
+      </c>
+      <c r="H145" t="s">
+        <v>26</v>
+      </c>
+      <c r="I145" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J145" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K145" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L145" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N145" s="5"/>
+    </row>
+    <row r="146" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>387</v>
+      </c>
+      <c r="B146">
+        <v>17</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D146" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H146" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I146" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J146" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K146" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L146" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N146" s="5"/>
+    </row>
+    <row r="147" spans="1:14" ht="68" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>18</v>
+      </c>
+      <c r="C147" t="s">
+        <v>13</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="G147" t="s">
+        <v>44</v>
+      </c>
+      <c r="H147" t="s">
+        <v>31</v>
+      </c>
+      <c r="I147" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J147" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K147" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="L147" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N147" s="5"/>
+    </row>
+    <row r="148" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>19</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D148" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="F148" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H148" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I148" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="J148" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K148" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L148" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N148" s="5"/>
+    </row>
+    <row r="149" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>20</v>
+      </c>
+      <c r="C149" t="s">
+        <v>13</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="G149" t="s">
+        <v>25</v>
+      </c>
+      <c r="H149" t="s">
+        <v>26</v>
+      </c>
+      <c r="I149" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J149" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K149" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L149" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N149" s="5"/>
+    </row>
+    <row r="150" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>21</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F150" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H150" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I150" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J150" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K150" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L150" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N150" s="5"/>
+    </row>
+    <row r="151" spans="1:14" ht="136" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>397</v>
+      </c>
+      <c r="B151">
+        <v>22</v>
+      </c>
+      <c r="C151" t="s">
+        <v>72</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F151" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="G151" t="s">
+        <v>17</v>
+      </c>
+      <c r="H151" t="s">
+        <v>18</v>
+      </c>
+      <c r="I151" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J151" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K151" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L151" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N151" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>